<commit_message>
Create script database for user detail
Database/[ITM]ScriptDatabase20150210.txt << create
Database/db-itm.xlsx << update
</commit_message>
<xml_diff>
--- a/Database/db-itm.xlsx
+++ b/Database/db-itm.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KU\2-2014\Information Technology Managment\ITM_Distance\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="787" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="787" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="สารบัญ" sheetId="8" r:id="rId1"/>
     <sheet name="CREATE" sheetId="9" r:id="rId2"/>
     <sheet name="INSERT" sheetId="10" r:id="rId3"/>
-    <sheet name="DROP,DELETE" sheetId="11" r:id="rId4"/>
-    <sheet name="user_detail" sheetId="1" r:id="rId5"/>
+    <sheet name="DELETE" sheetId="11" r:id="rId4"/>
+    <sheet name="master_amphur" sheetId="3" r:id="rId5"/>
     <sheet name="master_provine" sheetId="2" r:id="rId6"/>
-    <sheet name="master_amphur" sheetId="3" r:id="rId7"/>
-    <sheet name="master_tambon" sheetId="4" r:id="rId8"/>
-    <sheet name="role" sheetId="6" r:id="rId9"/>
-    <sheet name="status" sheetId="7" r:id="rId10"/>
+    <sheet name="master_tambon" sheetId="4" r:id="rId7"/>
+    <sheet name="role" sheetId="6" r:id="rId8"/>
+    <sheet name="status" sheetId="7" r:id="rId9"/>
+    <sheet name="user_detail" sheetId="1" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="185">
   <si>
     <t>id</t>
   </si>
@@ -86,9 +87,6 @@
     <t>INSERT</t>
   </si>
   <si>
-    <t>DROP,DELETE</t>
-  </si>
-  <si>
     <t>Command SQL</t>
   </si>
   <si>
@@ -369,6 +367,228 @@
   </si>
   <si>
     <t>อุบลราชธานี</t>
+  </si>
+  <si>
+    <t>Table Name</t>
+  </si>
+  <si>
+    <t>command</t>
+  </si>
+  <si>
+    <t>CREATE TABLE</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>serial</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>CONSTRAINT</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY</t>
+  </si>
+  <si>
+    <t>(id)</t>
+  </si>
+  <si>
+    <t>pk_master_province</t>
+  </si>
+  <si>
+    <t>character varying(64)</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>character varying(1024)</t>
+  </si>
+  <si>
+    <t>pid</t>
+  </si>
+  <si>
+    <t>character varying(128)</t>
+  </si>
+  <si>
+    <t>pk_role</t>
+  </si>
+  <si>
+    <t>pk_status</t>
+  </si>
+  <si>
+    <t>pk_user_detail</t>
+  </si>
+  <si>
+    <t>picture</t>
+  </si>
+  <si>
+    <t>character varying(255)</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>ALTER SEQEUNCE</t>
+  </si>
+  <si>
+    <t>DELETE FROM</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>RESTART WITH 1</t>
+  </si>
+  <si>
+    <t>master_amphur_id_seq</t>
+  </si>
+  <si>
+    <t>master_province_id_seq</t>
+  </si>
+  <si>
+    <t>master_tambon_id_seq</t>
+  </si>
+  <si>
+    <t>role_id_seq</t>
+  </si>
+  <si>
+    <t>status_id_seq</t>
+  </si>
+  <si>
+    <t>user_detail_id_seq</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>character varying(32)</t>
+  </si>
+  <si>
+    <t>INSERT INTO</t>
+  </si>
+  <si>
+    <t>VALUES</t>
+  </si>
+  <si>
+    <t>);</t>
+  </si>
+  <si>
+    <t>'Active'</t>
+  </si>
+  <si>
+    <t>'Inactive'</t>
+  </si>
+  <si>
+    <t>'Admin'</t>
+  </si>
+  <si>
+    <t>'User'</t>
+  </si>
+  <si>
+    <t>username,</t>
+  </si>
+  <si>
+    <t>password,</t>
+  </si>
+  <si>
+    <t>firstname,</t>
+  </si>
+  <si>
+    <t>lastname,</t>
+  </si>
+  <si>
+    <t>nickname,</t>
+  </si>
+  <si>
+    <t>role,</t>
+  </si>
+  <si>
+    <t>zodiac5432@gmail.com</t>
+  </si>
+  <si>
+    <t>hunjii4ni@gmail.com</t>
+  </si>
+  <si>
+    <t>0867853920</t>
+  </si>
+  <si>
+    <t>0824802535</t>
+  </si>
+  <si>
+    <t>2,</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>'pasoom',</t>
+  </si>
+  <si>
+    <t>'123456',</t>
+  </si>
+  <si>
+    <t>'Metis',</t>
+  </si>
+  <si>
+    <t>'Rattanachai',</t>
+  </si>
+  <si>
+    <t>'Oom',</t>
+  </si>
+  <si>
+    <t>'hunjii4ni@gmail.com',</t>
+  </si>
+  <si>
+    <t>'0824802535',</t>
+  </si>
+  <si>
+    <t>1,</t>
+  </si>
+  <si>
+    <t>email,</t>
+  </si>
+  <si>
+    <t>phone,</t>
+  </si>
+  <si>
+    <t>),</t>
+  </si>
+  <si>
+    <t>'paspond',</t>
+  </si>
+  <si>
+    <t>'Perapong',</t>
+  </si>
+  <si>
+    <t>'Soonketboon',</t>
+  </si>
+  <si>
+    <t>'Pond',</t>
+  </si>
+  <si>
+    <t>'zodiac5432@gmail.com',</t>
+  </si>
+  <si>
+    <t>'0867853920',</t>
   </si>
 </sst>
 </file>
@@ -400,7 +620,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -408,12 +628,181 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -424,7 +813,147 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -714,7 +1243,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,109 +1252,132 @@
     <col min="2" max="2" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="26">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="27"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="7">
+        <v>3</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
+        <v>2</v>
+      </c>
+      <c r="B5" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="1">
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="7">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="1">
+      <c r="D6" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="7">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="D7" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="7">
+        <v>4</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="7">
+        <v>5</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="7">
+        <v>6</v>
+      </c>
+      <c r="D10" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="1">
-        <v>3</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="1">
-        <v>4</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="1">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="1">
-        <v>6</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" location="CREATE!A1" display="CREATE"/>
+    <hyperlink ref="D3" location="INSERT!A1" display="INSERT"/>
+    <hyperlink ref="D4" location="DELETE!A1" display="DELETE"/>
+    <hyperlink ref="D5" location="master_amphur!A1" display="master_amphur"/>
+    <hyperlink ref="D6" location="master_provine!A1" display="master_province"/>
+    <hyperlink ref="D7" location="master_tambon!A1" display="master_tambon"/>
+    <hyperlink ref="D8" location="role!A1" display="role"/>
+    <hyperlink ref="D9" location="status!A1" display="status"/>
+    <hyperlink ref="D10" location="user_detail!A1" display="user_detail"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -836,108 +1388,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="4" tint="-0.499984740745262"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="4" tint="-0.499984740745262"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="4" tint="-0.499984740745262"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="9"/>
-  </sheetPr>
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B3" sqref="B3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,12 +1402,14 @@
     <col min="4" max="4" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -972,63 +1428,1658 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2">
-        <v>1</v>
+        <v>123456</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="G2" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" s="51" t="s">
+        <v>164</v>
+      </c>
+      <c r="I2" s="2">
         <v>2</v>
       </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2">
+        <v>123456</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>163</v>
+      </c>
+      <c r="H3" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="A11:I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2">
+        <v>123456</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>164</v>
+      </c>
+      <c r="H1" s="2">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="I1" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>CONCATENATE(A1,A2)</f>
+        <v>paspond,</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:I3" si="0">CONCATENATE(B1,B2)</f>
+        <v>123456,</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>Perapong,</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>Soonketboon,</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="0"/>
+        <v>Pond,</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v>zodiac5432@gmail.com,</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>0867853920,</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="0"/>
+        <v>2,</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="F7" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="H7" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="I7" s="52" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2">
+        <v>123456</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
+      <c r="F8" s="50" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="E9" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="F9" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>CONCATENATE(A7,A8,A9,A10,)</f>
+        <v>'pasoom',</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" ref="B11:I11" si="1">CONCATENATE(B7,B8,B9,B10,)</f>
+        <v>'123456',</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>'Metis',</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>'Rattanachai',</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>'Oom',</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
+        <v>'hunjii4ni@gmail.com',</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>'0824802535',</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
+        <v>'1,</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="1"/>
+        <v>'1,</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F1" r:id="rId1"/>
+    <hyperlink ref="F8" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:I35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>4</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="18"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>5</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="15"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>6</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H24" s="5"/>
+      <c r="I24" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H25" s="5"/>
+      <c r="I25" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H26" s="5"/>
+      <c r="I26" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="I27" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="H28" s="5"/>
+      <c r="I28" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="I30" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G31" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="H31" s="5"/>
+      <c r="I31" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H32" s="5"/>
+      <c r="I32" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H33" s="5"/>
+      <c r="I33" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:O10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="43"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="23">
+        <v>1</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="44"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="53"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="H4" s="40"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="54"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="23">
+        <v>2</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="38"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="53"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="53"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="H7" s="40"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="54"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="23">
+        <v>3</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="H9" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="I9" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="J9" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="K9" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="L9" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="M9" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="N9" s="36">
+        <v>1</v>
+      </c>
+      <c r="O9" s="53" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="G10" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="H10" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="I10" s="47" t="s">
+        <v>171</v>
+      </c>
+      <c r="J10" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="K10" s="47" t="s">
+        <v>173</v>
+      </c>
+      <c r="L10" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="M10" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="N10" s="39">
+        <v>1</v>
+      </c>
+      <c r="O10" s="54" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="20"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>1</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <v>2</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>3</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
+        <v>4</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>5</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <v>6</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="C1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1043,8 +3094,8 @@
   </sheetPr>
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,7 +3128,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="3">
         <v>99.020723349999997</v>
@@ -1094,7 +3145,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="3">
         <v>100.6253214</v>
@@ -1111,7 +3162,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3">
         <v>99.047880320000004</v>
@@ -1128,7 +3179,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="3">
         <v>103.6231339</v>
@@ -1145,7 +3196,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="3">
         <v>99.534323790000002</v>
@@ -1162,7 +3213,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="3">
         <v>102.5781898</v>
@@ -1179,7 +3230,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="3">
         <v>102.1308554</v>
@@ -1196,7 +3247,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3">
         <v>101.4429207</v>
@@ -1213,7 +3264,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3">
         <v>101.2016466</v>
@@ -1230,7 +3281,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="3">
         <v>100.0265062</v>
@@ -1247,7 +3298,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="3">
         <v>101.81395879999999</v>
@@ -1264,7 +3315,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3">
         <v>99.066003940000002</v>
@@ -1281,7 +3332,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="3">
         <v>99.869210879999997</v>
@@ -1298,7 +3349,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="3">
         <v>98.728865990000003</v>
@@ -1315,7 +3366,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="3">
         <v>99.609383170000001</v>
@@ -1332,7 +3383,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="3">
         <v>102.5221461</v>
@@ -1349,7 +3400,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="3">
         <v>98.792462970000003</v>
@@ -1366,7 +3417,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="3">
         <v>101.1732074</v>
@@ -1383,7 +3434,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="3">
         <v>100.1060516</v>
@@ -1400,7 +3451,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="3">
         <v>104.4321115</v>
@@ -1417,7 +3468,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="3">
         <v>102.1095899</v>
@@ -1434,7 +3485,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="3">
         <v>99.780826849999997</v>
@@ -1451,7 +3502,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="3">
         <v>100.1522004</v>
@@ -1468,7 +3519,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="3">
         <v>100.3971801</v>
@@ -1485,7 +3536,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="3">
         <v>101.71866470000001</v>
@@ -1502,7 +3553,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="3">
         <v>100.8327541</v>
@@ -1519,7 +3570,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="3">
         <v>103.651657</v>
@@ -1536,7 +3587,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="3">
         <v>102.9511466</v>
@@ -1553,7 +3604,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" s="3">
         <v>100.6857134</v>
@@ -1570,7 +3621,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" s="3">
         <v>99.635262800000007</v>
@@ -1587,7 +3638,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C32" s="3">
         <v>101.64731740000001</v>
@@ -1604,7 +3655,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C33" s="3">
         <v>101.34737459999999</v>
@@ -1621,7 +3672,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C34" s="3">
         <v>100.52309959999999</v>
@@ -1638,7 +3689,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="3">
         <v>100.1897479</v>
@@ -1655,7 +3706,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C36" s="3">
         <v>98.414813960000004</v>
@@ -1672,7 +3723,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C37" s="3">
         <v>100.06413089999999</v>
@@ -1689,7 +3740,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C38" s="3">
         <v>100.3429627</v>
@@ -1706,7 +3757,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="3">
         <v>100.5446015</v>
@@ -1723,7 +3774,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C40" s="3">
         <v>99.620950739999998</v>
@@ -1740,7 +3791,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="3">
         <v>101.1444558</v>
@@ -1757,7 +3808,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C42" s="3">
         <v>100.0668173</v>
@@ -1774,7 +3825,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C43" s="3">
         <v>98.346387309999997</v>
@@ -1791,7 +3842,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C44" s="3">
         <v>103.1669928</v>
@@ -1808,7 +3859,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C45" s="3">
         <v>104.5146371</v>
@@ -1825,7 +3876,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C46" s="3">
         <v>98.03114454</v>
@@ -1842,7 +3893,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C47" s="3">
         <v>104.3404329</v>
@@ -1859,7 +3910,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C48" s="3">
         <v>101.2280856</v>
@@ -1876,7 +3927,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C49" s="3">
         <v>103.8155175</v>
@@ -1893,7 +3944,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C50" s="3">
         <v>98.707472510000002</v>
@@ -1910,7 +3961,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C51" s="3">
         <v>101.4285878</v>
@@ -1927,7 +3978,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C52" s="3">
         <v>99.578066320000005</v>
@@ -1944,7 +3995,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C53" s="3">
         <v>100.897385</v>
@@ -1961,7 +4012,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C54" s="3">
         <v>99.512510570000003</v>
@@ -1978,7 +4029,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C55" s="3">
         <v>98.953845169999994</v>
@@ -1995,7 +4046,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C56" s="3">
         <v>101.63222620000001</v>
@@ -2012,7 +4063,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C57" s="3">
         <v>104.37002099999999</v>
@@ -2029,7 +4080,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C58" s="3">
         <v>103.8233343</v>
@@ -2046,7 +4097,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C59" s="3">
         <v>100.5387171</v>
@@ -2063,7 +4114,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C60" s="3">
         <v>99.92970803</v>
@@ -2080,7 +4131,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C61" s="3">
         <v>100.71062809999999</v>
@@ -2097,7 +4148,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C62" s="3">
         <v>99.953142749999998</v>
@@ -2114,7 +4165,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C63" s="3">
         <v>100.2141598</v>
@@ -2131,7 +4182,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C64" s="3">
         <v>102.3258826</v>
@@ -2148,7 +4199,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C65" s="3">
         <v>101.01429349999999</v>
@@ -2165,7 +4216,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C66" s="3">
         <v>100.34793759999999</v>
@@ -2182,7 +4233,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C67" s="3">
         <v>99.711978439999996</v>
@@ -2199,7 +4250,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C68" s="3">
         <v>99.891230559999997</v>
@@ -2216,7 +4267,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C69" s="3">
         <v>99.088690220000004</v>
@@ -2233,7 +4284,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C70" s="3">
         <v>103.65430379999999</v>
@@ -2250,7 +4301,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C71" s="3">
         <v>103.31576750000001</v>
@@ -2267,7 +4318,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C72" s="3">
         <v>102.3007731</v>
@@ -2284,7 +4335,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C73" s="3">
         <v>100.3487999</v>
@@ -2301,7 +4352,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C74" s="3">
         <v>104.7413962</v>
@@ -2318,7 +4369,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C75" s="3">
         <v>102.863311</v>
@@ -2335,7 +4386,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C76" s="3">
         <v>100.515366</v>
@@ -2352,7 +4403,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C77" s="3">
         <v>99.478170879999993</v>
@@ -2369,7 +4420,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C78" s="3">
         <v>105.111728</v>
@@ -2426,29 +4477,40 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2464,13 +4526,14 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2486,7 +4549,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2494,7 +4557,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>